<commit_message>
:sparkle: nuevo flujo accesso a plataforma
</commit_message>
<xml_diff>
--- a/Inputs/DESARROLLO/CursosCra/CURSOS_AULA_CRA.xlsx
+++ b/Inputs/DESARROLLO/CursosCra/CURSOS_AULA_CRA.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="80">
   <si>
     <t>courseId</t>
   </si>
@@ -76,6 +76,12 @@
     <t>CRA_CURSOB_AULA5</t>
   </si>
   <si>
+    <t>Plan de formación; Curso B - Aula 6</t>
+  </si>
+  <si>
+    <t>CURSOB_AULA6</t>
+  </si>
+  <si>
     <t>Plan de Formación; Curso C. Organización de espacios y ambiente de bibliotecas escolares - Aula 1</t>
   </si>
   <si>
@@ -106,6 +112,12 @@
     <t>CRA_CURSOG_AULA3</t>
   </si>
   <si>
+    <t>Plan de formación; Curso G - Decisiones basadas en evidencia para la mejora de la biblioteca escolar-Aula 4</t>
+  </si>
+  <si>
+    <t>CURSOG_AULA4</t>
+  </si>
+  <si>
     <t>Plan de Formación; Curso J : Vínculo con otras organizaciones de fomento del libro y la lectura -Aula 1</t>
   </si>
   <si>
@@ -176,14 +188,78 @@
   </si>
   <si>
     <t>CRA_CURSO0_AULA9</t>
+  </si>
+  <si>
+    <t>Plan de Formación: Tutorial- Aula 10</t>
+  </si>
+  <si>
+    <t>CRA_CURSO0_AULA10</t>
+  </si>
+  <si>
+    <t>Plan de Formación: Tutorial- Aula 11</t>
+  </si>
+  <si>
+    <t>CRA_CURSO0_AULA11</t>
+  </si>
+  <si>
+    <t>Plan de Formación: Tutorial- Aula 12</t>
+  </si>
+  <si>
+    <t>CRA_CURSO0_AULA12</t>
+  </si>
+  <si>
+    <t>Plan de Formación: Tutorial- Aula 13</t>
+  </si>
+  <si>
+    <t>CURSO0_AULA13</t>
+  </si>
+  <si>
+    <t>Plan de Formación; Curso F: Curiosidad, colaboración, creatividad y pensamiento crítico en la biblioteca - Aula 1</t>
+  </si>
+  <si>
+    <t>CRA_CURSOF_AULA1</t>
+  </si>
+  <si>
+    <t>Alto nivel de tutoría</t>
+  </si>
+  <si>
+    <t>Plan de Formación; Curso F: Curiosidad, colaboración, creatividad y pensamiento crítico en la biblioteca - Aula 2</t>
+  </si>
+  <si>
+    <t>CRA_CURSOF_AULA2</t>
+  </si>
+  <si>
+    <t>Plan de Formación; Curso E: Currículum escolar y fomento de la lectura- Aula 1</t>
+  </si>
+  <si>
+    <t>CRA_CURSOE_AULA1</t>
+  </si>
+  <si>
+    <t>Plan de Formación; Curso E: Currículum escolar y fomento de la lectura- Aula 2</t>
+  </si>
+  <si>
+    <t>CRA_CURSOE_AULA2</t>
+  </si>
+  <si>
+    <t>Plan de Formación; Curso H: Liderazgo del encargado de biblioteca en la comunidad escolar - Aula 1</t>
+  </si>
+  <si>
+    <t>CRA_CURSOH_AULA1</t>
+  </si>
+  <si>
+    <t>Plan de Formación; Curso H: Liderazgo del encargado de biblioteca en la comunidad escolar - Aula 2</t>
+  </si>
+  <si>
+    <t>CRA_CURSOH_AULA2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -191,11 +267,11 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -211,17 +287,23 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -449,16 +531,16 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -469,470 +551,720 @@
       <c r="A2" s="1">
         <v>10781.0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>44459.0</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="3">
+        <v>44484.0</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>10782.0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>44459.0</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="3">
+        <v>44484.0</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>10799.0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>44463.0</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="3">
+        <v>44828.0</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>10800.0</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>44463.0</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>44828.0</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>10801.0</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>44463.0</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>44828.0</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>10802.0</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>44463.0</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>44828.0</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>10803.0</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>44463.0</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>44828.0</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2">
+      <c r="A9" s="4">
+        <v>10819.0</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3">
+        <v>44478.0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>44843.0</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
         <v>10783.0</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="3">
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2">
         <v>44459.0</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2">
+      <c r="E10" s="2">
+        <v>44484.0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
         <v>10784.0</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="3">
+      <c r="B11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2">
         <v>44459.0</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2">
+      <c r="E11" s="2">
+        <v>44484.0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
         <v>10796.0</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="2">
         <v>44463.0</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E12" s="2">
         <v>44828.0</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2">
+      <c r="F12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
         <v>10797.0</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="3">
+      <c r="B13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="2">
         <v>44463.0</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E13" s="2">
         <v>44828.0</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2">
+      <c r="F13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
         <v>10798.0</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="3">
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="2">
         <v>44463.0</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E14" s="2">
         <v>44828.0</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2">
+      <c r="F14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>10817.0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="2">
+        <v>44463.0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>44828.0</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
         <v>10809.0</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="3">
+      <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="2">
         <v>44464.0</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E16" s="2">
         <v>44829.0</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2">
+      <c r="F16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
         <v>10810.0</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="3">
+      <c r="B17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="2">
         <v>44464.0</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E17" s="2">
         <v>44829.0</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2">
+      <c r="F17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
         <v>10811.0</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="3">
+      <c r="B18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="2">
         <v>44464.0</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E18" s="2">
         <v>44829.0</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2">
+      <c r="F18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
         <v>10778.0</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="3">
+      <c r="B19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="2">
         <v>44464.0</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E19" s="2">
         <v>44829.0</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2">
+      <c r="F19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
         <v>10779.0</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="3">
+      <c r="B20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="2">
         <v>44464.0</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E20" s="2">
         <v>44829.0</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2">
+      <c r="F20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
         <v>10780.0</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="3">
+      <c r="B21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="2">
         <v>44464.0</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E21" s="2">
         <v>44829.0</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2">
+      <c r="F21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
         <v>10804.0</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="3">
+      <c r="B22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="2">
         <v>44464.0</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E22" s="2">
         <v>44829.0</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2">
+      <c r="F22" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1">
         <v>10805.0</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="3">
+      <c r="B23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="2">
         <v>44464.0</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E23" s="2">
         <v>44829.0</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2">
+      <c r="F23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
         <v>10806.0</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="3">
+      <c r="B24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="2">
         <v>44464.0</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E24" s="2">
         <v>44829.0</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="2">
+      <c r="F24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
         <v>10807.0</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="3">
+      <c r="B25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="2">
         <v>44464.0</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E25" s="2">
         <v>44829.0</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="2">
+      <c r="F25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
         <v>10812.0</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="3">
+      <c r="B26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="2">
         <v>44464.0</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E26" s="2">
         <v>44829.0</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="2">
+      <c r="F26" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
         <v>10813.0</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="3">
+      <c r="B27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="2">
         <v>44464.0</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E27" s="2">
         <v>44829.0</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>8</v>
+      <c r="F27" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1">
+        <v>10822.0</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="5">
+        <v>44482.0</v>
+      </c>
+      <c r="E28" s="5">
+        <v>44847.0</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1">
+        <v>10823.0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="5">
+        <v>44482.0</v>
+      </c>
+      <c r="E29" s="5">
+        <v>44847.0</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1">
+        <v>10824.0</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="5">
+        <v>44482.0</v>
+      </c>
+      <c r="E30" s="5">
+        <v>44847.0</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1">
+        <v>10820.0</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="5">
+        <v>44478.0</v>
+      </c>
+      <c r="E31" s="5">
+        <v>44843.0</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1">
+        <v>10827.0</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D32" s="5">
+        <v>44482.0</v>
+      </c>
+      <c r="E32" s="5">
+        <v>44847.0</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1">
+        <v>10828.0</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="5">
+        <v>44482.0</v>
+      </c>
+      <c r="E33" s="5">
+        <v>44847.0</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1">
+        <v>10825.0</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="5">
+        <v>44482.0</v>
+      </c>
+      <c r="E34" s="5">
+        <v>44847.0</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1">
+        <v>10826.0</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" s="5">
+        <v>44482.0</v>
+      </c>
+      <c r="E35" s="5">
+        <v>44847.0</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1">
+        <v>10830.0</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="5">
+        <v>44483.0</v>
+      </c>
+      <c r="E36" s="5">
+        <v>44848.0</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1">
+        <v>10831.0</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" s="5">
+        <v>44483.0</v>
+      </c>
+      <c r="E37" s="5">
+        <v>44848.0</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:zap: Se agregan nuevas funcionalidades para extraer la data desde situación final
</commit_message>
<xml_diff>
--- a/Inputs/DESARROLLO/CursosCra/CURSOS_AULA_CRA.xlsx
+++ b/Inputs/DESARROLLO/CursosCra/CURSOS_AULA_CRA.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="110">
   <si>
     <t>courseId</t>
   </si>
@@ -46,6 +46,12 @@
     <t>CRA_CURSOA_AULA2</t>
   </si>
   <si>
+    <t>Plan de Formación; Curso A: ¿Qué es el Centro de lectura y biblioteca escolar (CRA)? Propósitos y servicios - Aula 3</t>
+  </si>
+  <si>
+    <t>CRA_CURSOA_AULA3</t>
+  </si>
+  <si>
     <t>Plan de formación; Curso B: Organización, catalogación y circulación de recursos de la biblioteca escolar - Aula 1</t>
   </si>
   <si>
@@ -82,6 +88,24 @@
     <t>CURSOB_AULA6</t>
   </si>
   <si>
+    <t>Plan de formación; Curso B: Organización, catalogación y circulación de recursos de la biblioteca escolar - Aula 7</t>
+  </si>
+  <si>
+    <t>CRA_CURSOB_AULA7</t>
+  </si>
+  <si>
+    <t>Plan de formación; Curso B: Organización, catalogación y circulación de recursos de la biblioteca escolar - Aula 8</t>
+  </si>
+  <si>
+    <t>CRA_CURSOB_AULA8</t>
+  </si>
+  <si>
+    <t>Plan de formación; Curso B: Organización, catalogación y circulación de recursos de la biblioteca escolar - Aula 9</t>
+  </si>
+  <si>
+    <t>CRA_CURSOB_AULA9</t>
+  </si>
+  <si>
     <t>Plan de Formación; Curso C. Organización de espacios y ambiente de bibliotecas escolares - Aula 1</t>
   </si>
   <si>
@@ -94,6 +118,51 @@
     <t>CRA_CURSOC_AULA2</t>
   </si>
   <si>
+    <t>Plan de Formación; Curso C. Organización de espacios y ambiente de bibliotecas escolares - Aula 3</t>
+  </si>
+  <si>
+    <t>CRA_CURSOC_AULA3</t>
+  </si>
+  <si>
+    <t>Plan de Formación; Curso D: Desarrollo de las colecciones - Aula 1</t>
+  </si>
+  <si>
+    <t>CRA_CURSOD_AULA1</t>
+  </si>
+  <si>
+    <t>Plan de Formación; Curso D: Desarrollo de las colecciones - Aula 2</t>
+  </si>
+  <si>
+    <t>CRA_CURSOD_AULA2</t>
+  </si>
+  <si>
+    <t>Plan de Formación; Curso E: Currículum escolar y fomento de la lectura- Aula 1</t>
+  </si>
+  <si>
+    <t>CRA_CURSOE_AULA1</t>
+  </si>
+  <si>
+    <t>Alto nivel de tutoría</t>
+  </si>
+  <si>
+    <t>Plan de Formación; Curso E: Currículum escolar y fomento de la lectura- Aula 2</t>
+  </si>
+  <si>
+    <t>CRA_CURSOE_AULA2</t>
+  </si>
+  <si>
+    <t>Plan de Formación; Curso F: Curiosidad, colaboración, creatividad y pensamiento crítico en la biblioteca - Aula 1</t>
+  </si>
+  <si>
+    <t>CRA_CURSOF_AULA1</t>
+  </si>
+  <si>
+    <t>Plan de Formación; Curso F: Curiosidad, colaboración, creatividad y pensamiento crítico en la biblioteca - Aula 2</t>
+  </si>
+  <si>
+    <t>CRA_CURSOF_AULA2</t>
+  </si>
+  <si>
     <t>Plan de formación; Curso G - Decisiones basadas en evidencia para la mejora de la biblioteca escolar-Aula 1</t>
   </si>
   <si>
@@ -118,6 +187,30 @@
     <t>CURSOG_AULA4</t>
   </si>
   <si>
+    <t>Plan de Formación; Curso H: Liderazgo del encargado de biblioteca en la comunidad escolar - Aula 1</t>
+  </si>
+  <si>
+    <t>CRA_CURSOH_AULA1</t>
+  </si>
+  <si>
+    <t>Plan de Formación; Curso H: Liderazgo del encargado de biblioteca en la comunidad escolar - Aula 2</t>
+  </si>
+  <si>
+    <t>CRA_CURSOH_AULA2</t>
+  </si>
+  <si>
+    <t>Plan de Formación; Curso I:Promoción de la lectura en la comunidad escolar - Aula 1</t>
+  </si>
+  <si>
+    <t>CRA_CURSOI_AULA1</t>
+  </si>
+  <si>
+    <t>Plan de Formación; Curso I:Promoción de la lectura en la comunidad escolar - Aula 2</t>
+  </si>
+  <si>
+    <t>CRA_CURSOI_AULA2</t>
+  </si>
+  <si>
     <t>Plan de Formación; Curso J : Vínculo con otras organizaciones de fomento del libro y la lectura -Aula 1</t>
   </si>
   <si>
@@ -136,121 +229,118 @@
     <t>CRA_CURSOJ_AULA3</t>
   </si>
   <si>
-    <t>Plan de Formación: Tutorial- Aula 1</t>
+    <t>Plan de Formación: Curso J - Aula 4</t>
+  </si>
+  <si>
+    <t>CURSOJ_AULA4</t>
+  </si>
+  <si>
+    <t>Curso 0 o Tutorial - Aula 1</t>
   </si>
   <si>
     <t>CRA_CURSO0_AULA1</t>
   </si>
   <si>
-    <t>Plan de Formación: Tutorial- Aula 2</t>
+    <t>Curso 0 o Tutorial - Aula 2</t>
   </si>
   <si>
     <t>CRA_CURSO0_AULA2</t>
   </si>
   <si>
-    <t>Plan de Formación: Tutorial- Aula 3</t>
+    <t>Curso 0 o Tutorial - Aula 3</t>
   </si>
   <si>
     <t>CRA_CURSO0_AULA3</t>
   </si>
   <si>
-    <t>Plan de Formación: Tutorial- Aula 4</t>
+    <t>Curso 0 o Tutorial - Aula 4</t>
   </si>
   <si>
     <t>CRA_CURSO0_AULA4</t>
   </si>
   <si>
-    <t>Plan de Formación: Tutorial- Aula 5</t>
+    <t>Curso 0 o Tutorial - Aula 5</t>
   </si>
   <si>
     <t>CRA_CURSO0_AULA5</t>
   </si>
   <si>
-    <t>Plan de Formación: Tutorial- Aula 6</t>
+    <t>Curso 0 o Tutorial - Aula 6</t>
   </si>
   <si>
     <t>CRA_CURSO0_AULA6</t>
   </si>
   <si>
-    <t>Plan de Formación: Tutorial- Aula 7</t>
+    <t>Curso 0 o Tutorial - Aula 7</t>
   </si>
   <si>
     <t>CRA_CURSO0_AULA7</t>
   </si>
   <si>
-    <t>Plan de Formación: Tutorial- Aula 8</t>
+    <t>Curso 0 o Tutorial - Aula 8</t>
   </si>
   <si>
     <t>CRA_CURSO0_AULA8</t>
   </si>
   <si>
-    <t>Plan de Formación: Tutorial- Aula 9</t>
+    <t>Curso 0 o Tutorial - Aula 9</t>
   </si>
   <si>
     <t>CRA_CURSO0_AULA9</t>
   </si>
   <si>
-    <t>Plan de Formación: Tutorial- Aula 10</t>
+    <t>Curso 0 o Tutorial - Aula 10</t>
   </si>
   <si>
     <t>CRA_CURSO0_AULA10</t>
   </si>
   <si>
-    <t>Plan de Formación: Tutorial- Aula 11</t>
+    <t>Curso 0 o Tutorial - Aula 11</t>
   </si>
   <si>
     <t>CRA_CURSO0_AULA11</t>
   </si>
   <si>
-    <t>Plan de Formación: Tutorial- Aula 12</t>
+    <t>Curso 0 o Tutorial - Aula 12</t>
   </si>
   <si>
     <t>CRA_CURSO0_AULA12</t>
   </si>
   <si>
-    <t>Plan de Formación: Tutorial- Aula 13</t>
+    <t>Curso 0 o Tutorial - Aula 13</t>
   </si>
   <si>
     <t>CURSO0_AULA13</t>
   </si>
   <si>
-    <t>Plan de Formación; Curso F: Curiosidad, colaboración, creatividad y pensamiento crítico en la biblioteca - Aula 1</t>
-  </si>
-  <si>
-    <t>CRA_CURSOF_AULA1</t>
-  </si>
-  <si>
-    <t>Alto nivel de tutoría</t>
-  </si>
-  <si>
-    <t>Plan de Formación; Curso F: Curiosidad, colaboración, creatividad y pensamiento crítico en la biblioteca - Aula 2</t>
-  </si>
-  <si>
-    <t>CRA_CURSOF_AULA2</t>
-  </si>
-  <si>
-    <t>Plan de Formación; Curso E: Currículum escolar y fomento de la lectura- Aula 1</t>
-  </si>
-  <si>
-    <t>CRA_CURSOE_AULA1</t>
-  </si>
-  <si>
-    <t>Plan de Formación; Curso E: Currículum escolar y fomento de la lectura- Aula 2</t>
-  </si>
-  <si>
-    <t>CRA_CURSOE_AULA2</t>
-  </si>
-  <si>
-    <t>Plan de Formación; Curso H: Liderazgo del encargado de biblioteca en la comunidad escolar - Aula 1</t>
-  </si>
-  <si>
-    <t>CRA_CURSOH_AULA1</t>
-  </si>
-  <si>
-    <t>Plan de Formación; Curso H: Liderazgo del encargado de biblioteca en la comunidad escolar - Aula 2</t>
-  </si>
-  <si>
-    <t>CRA_CURSOH_AULA2</t>
+    <t>Curso 0 o Tutorial - Aula 14</t>
+  </si>
+  <si>
+    <t>CRA_CURSO0_AULA14</t>
+  </si>
+  <si>
+    <t>Curso 0 o Tutorial - Aula 15</t>
+  </si>
+  <si>
+    <t>CRA_CURSO0_AULA15</t>
+  </si>
+  <si>
+    <t>Curso 0 o Tutorial - Aula 16</t>
+  </si>
+  <si>
+    <t>CRA_CURSO0_AULA16</t>
+  </si>
+  <si>
+    <t>Curso 0 o Tutorial - Aula 17</t>
+  </si>
+  <si>
+    <t>CRA_CURSO0_AULA17</t>
+  </si>
+  <si>
+    <t>Curso 0 o Tutorial - Aula 18</t>
+  </si>
+  <si>
+    <t>CRA_CURSO0_AULA18</t>
   </si>
 </sst>
 </file>
@@ -287,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -297,13 +387,16 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -523,7 +616,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="100.14"/>
-    <col customWidth="1" min="3" max="3" width="21.43"/>
+    <col customWidth="1" min="3" max="3" width="22.29"/>
     <col customWidth="1" min="4" max="4" width="17.71"/>
   </cols>
   <sheetData>
@@ -560,8 +653,8 @@
       <c r="D2" s="2">
         <v>44459.0</v>
       </c>
-      <c r="E2" s="3">
-        <v>44484.0</v>
+      <c r="E2" s="2">
+        <v>44508.0</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
@@ -580,8 +673,8 @@
       <c r="D3" s="2">
         <v>44459.0</v>
       </c>
-      <c r="E3" s="3">
-        <v>44484.0</v>
+      <c r="E3" s="2">
+        <v>44508.0</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -589,7 +682,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>10799.0</v>
+        <v>10839.0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -597,11 +690,9 @@
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2">
-        <v>44463.0</v>
-      </c>
-      <c r="E4" s="3">
-        <v>44828.0</v>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>44508.0</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>8</v>
@@ -609,7 +700,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>10800.0</v>
+        <v>10799.0</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
@@ -621,7 +712,7 @@
         <v>44463.0</v>
       </c>
       <c r="E5" s="2">
-        <v>44828.0</v>
+        <v>44508.0</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>8</v>
@@ -629,7 +720,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>10801.0</v>
+        <v>10800.0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>15</v>
@@ -641,7 +732,7 @@
         <v>44463.0</v>
       </c>
       <c r="E6" s="2">
-        <v>44828.0</v>
+        <v>44508.0</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>8</v>
@@ -649,7 +740,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>10802.0</v>
+        <v>10801.0</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>17</v>
@@ -661,7 +752,7 @@
         <v>44463.0</v>
       </c>
       <c r="E7" s="2">
-        <v>44828.0</v>
+        <v>44508.0</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>
@@ -669,7 +760,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>10803.0</v>
+        <v>10802.0</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>19</v>
@@ -681,27 +772,27 @@
         <v>44463.0</v>
       </c>
       <c r="E8" s="2">
-        <v>44828.0</v>
+        <v>44508.0</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4">
-        <v>10819.0</v>
+      <c r="A9" s="1">
+        <v>10803.0</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="3">
-        <v>44478.0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>44843.0</v>
+      <c r="D9" s="2">
+        <v>44463.0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>44508.0</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>8</v>
@@ -709,7 +800,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>10783.0</v>
+        <v>10819.0</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
@@ -718,10 +809,10 @@
         <v>24</v>
       </c>
       <c r="D10" s="2">
-        <v>44459.0</v>
+        <v>44478.0</v>
       </c>
       <c r="E10" s="2">
-        <v>44484.0</v>
+        <v>44508.0</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>8</v>
@@ -729,7 +820,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>10784.0</v>
+        <v>10840.0</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>25</v>
@@ -738,10 +829,10 @@
         <v>26</v>
       </c>
       <c r="D11" s="2">
-        <v>44459.0</v>
+        <v>44495.0</v>
       </c>
       <c r="E11" s="2">
-        <v>44484.0</v>
+        <v>44508.0</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>8</v>
@@ -749,7 +840,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>10796.0</v>
+        <v>10841.0</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>27</v>
@@ -758,10 +849,10 @@
         <v>28</v>
       </c>
       <c r="D12" s="2">
-        <v>44463.0</v>
+        <v>44495.0</v>
       </c>
       <c r="E12" s="2">
-        <v>44828.0</v>
+        <v>44508.0</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>8</v>
@@ -769,7 +860,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>10797.0</v>
+        <v>10842.0</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>29</v>
@@ -778,10 +869,10 @@
         <v>30</v>
       </c>
       <c r="D13" s="2">
-        <v>44463.0</v>
+        <v>44495.0</v>
       </c>
       <c r="E13" s="2">
-        <v>44828.0</v>
+        <v>44508.0</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>8</v>
@@ -789,7 +880,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>10798.0</v>
+        <v>10783.0</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>31</v>
@@ -798,10 +889,10 @@
         <v>32</v>
       </c>
       <c r="D14" s="2">
-        <v>44463.0</v>
+        <v>44459.0</v>
       </c>
       <c r="E14" s="2">
-        <v>44828.0</v>
+        <v>44508.0</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>8</v>
@@ -809,7 +900,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>10817.0</v>
+        <v>10784.0</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>33</v>
@@ -818,10 +909,10 @@
         <v>34</v>
       </c>
       <c r="D15" s="2">
-        <v>44463.0</v>
+        <v>44459.0</v>
       </c>
       <c r="E15" s="2">
-        <v>44828.0</v>
+        <v>44508.0</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>8</v>
@@ -829,7 +920,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>10809.0</v>
+        <v>10843.0</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>35</v>
@@ -838,10 +929,10 @@
         <v>36</v>
       </c>
       <c r="D16" s="2">
-        <v>44464.0</v>
+        <v>44477.0</v>
       </c>
       <c r="E16" s="2">
-        <v>44829.0</v>
+        <v>44508.0</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>8</v>
@@ -849,7 +940,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1">
-        <v>10810.0</v>
+        <v>10845.0</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>37</v>
@@ -858,18 +949,16 @@
         <v>38</v>
       </c>
       <c r="D17" s="2">
-        <v>44464.0</v>
+        <v>44508.0</v>
       </c>
       <c r="E17" s="2">
-        <v>44829.0</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>44547.0</v>
+      </c>
+      <c r="F17" s="1"/>
     </row>
     <row r="18">
       <c r="A18" s="1">
-        <v>10811.0</v>
+        <v>10846.0</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>39</v>
@@ -878,18 +967,16 @@
         <v>40</v>
       </c>
       <c r="D18" s="2">
-        <v>44464.0</v>
+        <v>44508.0</v>
       </c>
       <c r="E18" s="2">
-        <v>44829.0</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>44547.0</v>
+      </c>
+      <c r="F18" s="1"/>
     </row>
     <row r="19">
       <c r="A19" s="1">
-        <v>10778.0</v>
+        <v>10825.0</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>41</v>
@@ -897,91 +984,91 @@
       <c r="C19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="2">
-        <v>44464.0</v>
+      <c r="D19" s="3">
+        <v>44482.0</v>
       </c>
       <c r="E19" s="2">
-        <v>44829.0</v>
+        <v>44545.0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1">
-        <v>10779.0</v>
+        <v>10826.0</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="3">
+        <v>44482.0</v>
+      </c>
+      <c r="E20" s="2">
+        <v>44545.0</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="2">
-        <v>44464.0</v>
-      </c>
-      <c r="E20" s="2">
-        <v>44829.0</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1">
-        <v>10780.0</v>
+        <v>10827.0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="2">
-        <v>44464.0</v>
+        <v>47</v>
+      </c>
+      <c r="D21" s="3">
+        <v>44482.0</v>
       </c>
       <c r="E21" s="2">
-        <v>44829.0</v>
+        <v>44545.0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1">
-        <v>10804.0</v>
+        <v>10828.0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="2">
-        <v>44464.0</v>
+        <v>49</v>
+      </c>
+      <c r="D22" s="3">
+        <v>44482.0</v>
       </c>
       <c r="E22" s="2">
-        <v>44829.0</v>
+        <v>44545.0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1">
-        <v>10805.0</v>
+        <v>10796.0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D23" s="2">
-        <v>44464.0</v>
+        <v>44463.0</v>
       </c>
       <c r="E23" s="2">
-        <v>44829.0</v>
+        <v>44828.0</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>8</v>
@@ -989,19 +1076,19 @@
     </row>
     <row r="24">
       <c r="A24" s="1">
-        <v>10806.0</v>
+        <v>10797.0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D24" s="2">
-        <v>44464.0</v>
+        <v>44463.0</v>
       </c>
       <c r="E24" s="2">
-        <v>44829.0</v>
+        <v>44828.0</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>8</v>
@@ -1009,19 +1096,19 @@
     </row>
     <row r="25">
       <c r="A25" s="1">
-        <v>10807.0</v>
+        <v>10798.0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D25" s="2">
-        <v>44464.0</v>
+        <v>44463.0</v>
       </c>
       <c r="E25" s="2">
-        <v>44829.0</v>
+        <v>44828.0</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>8</v>
@@ -1029,119 +1116,111 @@
     </row>
     <row r="26">
       <c r="A26" s="1">
-        <v>10812.0</v>
+        <v>10817.0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D26" s="2">
-        <v>44464.0</v>
+        <v>44463.0</v>
       </c>
       <c r="E26" s="2">
-        <v>44829.0</v>
+        <v>44828.0</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1">
-        <v>10813.0</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="A27" s="4">
+        <v>10830.0</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="2">
-        <v>44464.0</v>
-      </c>
-      <c r="E27" s="2">
-        <v>44829.0</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>8</v>
+      <c r="C27" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="5">
+        <v>44483.0</v>
+      </c>
+      <c r="E27" s="6">
+        <v>44545.0</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1">
-        <v>10822.0</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="A28" s="4">
+        <v>10831.0</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>60</v>
       </c>
+      <c r="C28" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="D28" s="5">
-        <v>44482.0</v>
-      </c>
-      <c r="E28" s="5">
-        <v>44847.0</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>8</v>
+        <v>44483.0</v>
+      </c>
+      <c r="E28" s="6">
+        <v>44545.0</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1">
-        <v>10823.0</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="A29" s="4">
+        <v>10848.0</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="5">
-        <v>44482.0</v>
-      </c>
-      <c r="E29" s="5">
-        <v>44847.0</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="C29" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="6">
+        <v>44547.0</v>
+      </c>
+      <c r="F29" s="1"/>
     </row>
     <row r="30">
-      <c r="A30" s="1">
-        <v>10824.0</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="A30" s="4">
+        <v>10849.0</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D30" s="5">
-        <v>44482.0</v>
-      </c>
-      <c r="E30" s="5">
-        <v>44847.0</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="C30" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="6">
+        <v>44547.0</v>
+      </c>
+      <c r="F30" s="1"/>
     </row>
     <row r="31">
       <c r="A31" s="1">
-        <v>10820.0</v>
+        <v>10809.0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="5">
-        <v>44478.0</v>
-      </c>
-      <c r="E31" s="5">
-        <v>44843.0</v>
+        <v>67</v>
+      </c>
+      <c r="D31" s="2">
+        <v>44464.0</v>
+      </c>
+      <c r="E31" s="2">
+        <v>44829.0</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>8</v>
@@ -1149,27 +1228,27 @@
     </row>
     <row r="32">
       <c r="A32" s="1">
-        <v>10827.0</v>
+        <v>10810.0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="5">
-        <v>44482.0</v>
-      </c>
-      <c r="E32" s="5">
-        <v>44847.0</v>
-      </c>
-      <c r="F32" s="4" t="s">
         <v>69</v>
+      </c>
+      <c r="D32" s="2">
+        <v>44464.0</v>
+      </c>
+      <c r="E32" s="2">
+        <v>44829.0</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1">
-        <v>10828.0</v>
+        <v>10811.0</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>70</v>
@@ -1177,19 +1256,19 @@
       <c r="C33" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="5">
-        <v>44482.0</v>
-      </c>
-      <c r="E33" s="5">
-        <v>44847.0</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>69</v>
+      <c r="D33" s="2">
+        <v>44464.0</v>
+      </c>
+      <c r="E33" s="2">
+        <v>44829.0</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1">
-        <v>10825.0</v>
+        <v>10818.0</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>72</v>
@@ -1197,74 +1276,374 @@
       <c r="C34" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D34" s="5">
-        <v>44482.0</v>
-      </c>
-      <c r="E34" s="5">
-        <v>44847.0</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>69</v>
+      <c r="D34" s="3">
+        <v>44478.0</v>
+      </c>
+      <c r="E34" s="3">
+        <v>44843.0</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1">
-        <v>10826.0</v>
-      </c>
-      <c r="B35" s="1" t="s">
+        <v>10778.0</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>74</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D35" s="5">
-        <v>44482.0</v>
-      </c>
-      <c r="E35" s="5">
-        <v>44847.0</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>69</v>
+      <c r="D35" s="2">
+        <v>44464.0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>44829.0</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1">
-        <v>10830.0</v>
-      </c>
-      <c r="B36" s="1" t="s">
+        <v>10779.0</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D36" s="5">
-        <v>44483.0</v>
-      </c>
-      <c r="E36" s="5">
-        <v>44848.0</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>69</v>
+      <c r="D36" s="2">
+        <v>44464.0</v>
+      </c>
+      <c r="E36" s="2">
+        <v>44829.0</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1">
-        <v>10831.0</v>
-      </c>
-      <c r="B37" s="1" t="s">
+        <v>10780.0</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>78</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D37" s="5">
-        <v>44483.0</v>
-      </c>
-      <c r="E37" s="5">
-        <v>44848.0</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>69</v>
+      <c r="D37" s="2">
+        <v>44464.0</v>
+      </c>
+      <c r="E37" s="2">
+        <v>44829.0</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1">
+        <v>10804.0</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="2">
+        <v>44464.0</v>
+      </c>
+      <c r="E38" s="2">
+        <v>44829.0</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1">
+        <v>10805.0</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="2">
+        <v>44464.0</v>
+      </c>
+      <c r="E39" s="2">
+        <v>44829.0</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1">
+        <v>10806.0</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="2">
+        <v>44464.0</v>
+      </c>
+      <c r="E40" s="2">
+        <v>44829.0</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1">
+        <v>10807.0</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" s="2">
+        <v>44464.0</v>
+      </c>
+      <c r="E41" s="2">
+        <v>44829.0</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1">
+        <v>10812.0</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="2">
+        <v>44464.0</v>
+      </c>
+      <c r="E42" s="2">
+        <v>44829.0</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1">
+        <v>10813.0</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="2">
+        <v>44464.0</v>
+      </c>
+      <c r="E43" s="2">
+        <v>44829.0</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1">
+        <v>10822.0</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="3">
+        <v>44482.0</v>
+      </c>
+      <c r="E44" s="3">
+        <v>44847.0</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1">
+        <v>10823.0</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D45" s="3">
+        <v>44482.0</v>
+      </c>
+      <c r="E45" s="3">
+        <v>44847.0</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1">
+        <v>10824.0</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" s="3">
+        <v>44482.0</v>
+      </c>
+      <c r="E46" s="3">
+        <v>44847.0</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1">
+        <v>10820.0</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="3">
+        <v>44478.0</v>
+      </c>
+      <c r="E47" s="3">
+        <v>44843.0</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="4">
+        <v>10834.0</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="4">
+        <v>10835.0</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="4">
+        <v>10836.0</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="4">
+        <v>10837.0</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="4">
+        <v>10838.0</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="F54" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="F55" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
:recycle: Refactorizando los dirs y algunos flujos actualizados
</commit_message>
<xml_diff>
--- a/Inputs/DESARROLLO/CursosCra/CURSOS_AULA_CRA.xlsx
+++ b/Inputs/DESARROLLO/CursosCra/CURSOS_AULA_CRA.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="106">
   <si>
     <t>courseId</t>
   </si>
@@ -130,12 +130,6 @@
     <t>CRA_CURSOD_AULA1</t>
   </si>
   <si>
-    <t>Plan de Formación; Curso D: Desarrollo de las colecciones - Aula 2</t>
-  </si>
-  <si>
-    <t>CRA_CURSOD_AULA2</t>
-  </si>
-  <si>
     <t>Plan de Formación; Curso E: Currículum escolar y fomento de la lectura- Aula 1</t>
   </si>
   <si>
@@ -203,12 +197,6 @@
   </si>
   <si>
     <t>CRA_CURSOI_AULA1</t>
-  </si>
-  <si>
-    <t>Plan de Formación; Curso I:Promoción de la lectura en la comunidad escolar - Aula 2</t>
-  </si>
-  <si>
-    <t>CRA_CURSOI_AULA2</t>
   </si>
   <si>
     <t>Plan de Formación; Curso J : Vínculo con otras organizaciones de fomento del libro y la lectura -Aula 1</t>
@@ -958,7 +946,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1">
-        <v>10846.0</v>
+        <v>10825.0</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>39</v>
@@ -966,23 +954,25 @@
       <c r="C18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="2">
-        <v>44508.0</v>
+      <c r="D18" s="3">
+        <v>44482.0</v>
       </c>
       <c r="E18" s="2">
-        <v>44547.0</v>
-      </c>
-      <c r="F18" s="1"/>
+        <v>44545.0</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1">
-        <v>10825.0</v>
+        <v>10826.0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D19" s="3">
         <v>44482.0</v>
@@ -991,12 +981,12 @@
         <v>44545.0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1">
-        <v>10826.0</v>
+        <v>10827.0</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>44</v>
@@ -1011,12 +1001,12 @@
         <v>44545.0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1">
-        <v>10827.0</v>
+        <v>10828.0</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>46</v>
@@ -1031,12 +1021,12 @@
         <v>44545.0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1">
-        <v>10828.0</v>
+        <v>10796.0</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>48</v>
@@ -1044,19 +1034,19 @@
       <c r="C22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="3">
-        <v>44482.0</v>
+      <c r="D22" s="2">
+        <v>44463.0</v>
       </c>
       <c r="E22" s="2">
-        <v>44545.0</v>
+        <v>44828.0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1">
-        <v>10796.0</v>
+        <v>10797.0</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>50</v>
@@ -1076,7 +1066,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1">
-        <v>10797.0</v>
+        <v>10798.0</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>52</v>
@@ -1096,7 +1086,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1">
-        <v>10798.0</v>
+        <v>10817.0</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>54</v>
@@ -1115,28 +1105,28 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1">
-        <v>10817.0</v>
-      </c>
-      <c r="B26" s="1" t="s">
+      <c r="A26" s="4">
+        <v>10830.0</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="2">
-        <v>44463.0</v>
-      </c>
-      <c r="E26" s="2">
-        <v>44828.0</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>8</v>
+      <c r="D26" s="5">
+        <v>44483.0</v>
+      </c>
+      <c r="E26" s="6">
+        <v>44545.0</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4">
-        <v>10830.0</v>
+        <v>10831.0</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>58</v>
@@ -1151,12 +1141,12 @@
         <v>44545.0</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4">
-        <v>10831.0</v>
+        <v>10848.0</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>60</v>
@@ -1164,51 +1154,55 @@
       <c r="C28" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D28" s="5">
-        <v>44483.0</v>
-      </c>
+      <c r="D28" s="2"/>
       <c r="E28" s="6">
-        <v>44545.0</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>43</v>
-      </c>
+        <v>44547.0</v>
+      </c>
+      <c r="F28" s="1"/>
     </row>
     <row r="29">
-      <c r="A29" s="4">
-        <v>10848.0</v>
-      </c>
-      <c r="B29" s="4" t="s">
+      <c r="A29" s="1">
+        <v>10809.0</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="6">
-        <v>44547.0</v>
-      </c>
-      <c r="F29" s="1"/>
+      <c r="D29" s="2">
+        <v>44464.0</v>
+      </c>
+      <c r="E29" s="2">
+        <v>44829.0</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="4">
-        <v>10849.0</v>
-      </c>
-      <c r="B30" s="4" t="s">
+      <c r="A30" s="1">
+        <v>10810.0</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="6">
-        <v>44547.0</v>
-      </c>
-      <c r="F30" s="1"/>
+      <c r="D30" s="2">
+        <v>44464.0</v>
+      </c>
+      <c r="E30" s="2">
+        <v>44829.0</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1">
-        <v>10809.0</v>
+        <v>10811.0</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>66</v>
@@ -1228,7 +1222,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1">
-        <v>10810.0</v>
+        <v>10818.0</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>68</v>
@@ -1236,11 +1230,11 @@
       <c r="C32" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D32" s="2">
-        <v>44464.0</v>
-      </c>
-      <c r="E32" s="2">
-        <v>44829.0</v>
+      <c r="D32" s="3">
+        <v>44478.0</v>
+      </c>
+      <c r="E32" s="3">
+        <v>44843.0</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>8</v>
@@ -1248,9 +1242,9 @@
     </row>
     <row r="33">
       <c r="A33" s="1">
-        <v>10811.0</v>
-      </c>
-      <c r="B33" s="1" t="s">
+        <v>10778.0</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1268,19 +1262,19 @@
     </row>
     <row r="34">
       <c r="A34" s="1">
-        <v>10818.0</v>
-      </c>
-      <c r="B34" s="1" t="s">
+        <v>10779.0</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D34" s="3">
-        <v>44478.0</v>
-      </c>
-      <c r="E34" s="3">
-        <v>44843.0</v>
+      <c r="D34" s="2">
+        <v>44464.0</v>
+      </c>
+      <c r="E34" s="2">
+        <v>44829.0</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>8</v>
@@ -1288,7 +1282,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1">
-        <v>10778.0</v>
+        <v>10780.0</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>74</v>
@@ -1308,7 +1302,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1">
-        <v>10779.0</v>
+        <v>10804.0</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>76</v>
@@ -1328,7 +1322,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1">
-        <v>10780.0</v>
+        <v>10805.0</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>78</v>
@@ -1348,7 +1342,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1">
-        <v>10804.0</v>
+        <v>10806.0</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>80</v>
@@ -1368,7 +1362,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1">
-        <v>10805.0</v>
+        <v>10807.0</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>82</v>
@@ -1388,7 +1382,7 @@
     </row>
     <row r="40">
       <c r="A40" s="1">
-        <v>10806.0</v>
+        <v>10812.0</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>84</v>
@@ -1408,7 +1402,7 @@
     </row>
     <row r="41">
       <c r="A41" s="1">
-        <v>10807.0</v>
+        <v>10813.0</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>86</v>
@@ -1428,7 +1422,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1">
-        <v>10812.0</v>
+        <v>10822.0</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>88</v>
@@ -1436,11 +1430,11 @@
       <c r="C42" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="2">
-        <v>44464.0</v>
-      </c>
-      <c r="E42" s="2">
-        <v>44829.0</v>
+      <c r="D42" s="3">
+        <v>44482.0</v>
+      </c>
+      <c r="E42" s="3">
+        <v>44847.0</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>8</v>
@@ -1448,7 +1442,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1">
-        <v>10813.0</v>
+        <v>10823.0</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>90</v>
@@ -1456,11 +1450,11 @@
       <c r="C43" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D43" s="2">
-        <v>44464.0</v>
-      </c>
-      <c r="E43" s="2">
-        <v>44829.0</v>
+      <c r="D43" s="3">
+        <v>44482.0</v>
+      </c>
+      <c r="E43" s="3">
+        <v>44847.0</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>8</v>
@@ -1468,7 +1462,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1">
-        <v>10822.0</v>
+        <v>10824.0</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>92</v>
@@ -1488,7 +1482,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1">
-        <v>10823.0</v>
+        <v>10820.0</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>94</v>
@@ -1497,58 +1491,50 @@
         <v>95</v>
       </c>
       <c r="D45" s="3">
-        <v>44482.0</v>
+        <v>44478.0</v>
       </c>
       <c r="E45" s="3">
-        <v>44847.0</v>
+        <v>44843.0</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1">
-        <v>10824.0</v>
+      <c r="A46" s="4">
+        <v>10834.0</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D46" s="3">
-        <v>44482.0</v>
-      </c>
-      <c r="E46" s="3">
-        <v>44847.0</v>
-      </c>
-      <c r="F46" s="1" t="s">
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1">
-        <v>10820.0</v>
+      <c r="A47" s="4">
+        <v>10835.0</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D47" s="3">
-        <v>44478.0</v>
-      </c>
-      <c r="E47" s="3">
-        <v>44843.0</v>
-      </c>
-      <c r="F47" s="1" t="s">
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="4">
-        <v>10834.0</v>
+        <v>10836.0</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>100</v>
@@ -1564,7 +1550,7 @@
     </row>
     <row r="49">
       <c r="A49" s="4">
-        <v>10835.0</v>
+        <v>10837.0</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>102</v>
@@ -1580,7 +1566,7 @@
     </row>
     <row r="50">
       <c r="A50" s="4">
-        <v>10836.0</v>
+        <v>10838.0</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>104</v>
@@ -1595,15 +1581,9 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="4">
-        <v>10837.0</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>107</v>
-      </c>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="4" t="s">
@@ -1611,38 +1591,12 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="4">
-        <v>10838.0</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="4" t="s">
+      <c r="F52" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="F54" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="F55" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>